<commit_message>
Added new solid new datasource for the toolkit: US Bureau of economic analysis (BEA). New folder added in the backend that has a module for pulling BEA data and a GUI made with tkinter that eases the process of finding, charting and downloading BEA data. Still early version, only working with NIPA dataset thus far but will be developed further.
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
+++ b/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1074"/>
+  <dimension ref="A1:B1075"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9036,6 +9036,14 @@
       </c>
       <c r="B1074" t="n">
         <v>-76.292</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" s="3" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B1075" t="n">
+        <v>-77.74299999999999</v>
       </c>
     </row>
   </sheetData>
@@ -9084,7 +9092,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-07-09</t>
+          <t>2023-07-20</t>
         </is>
       </c>
     </row>
@@ -9096,7 +9104,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-07-09</t>
+          <t>2023-07-20</t>
         </is>
       </c>
     </row>
@@ -9132,7 +9140,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-07-05</t>
+          <t>2023-07-12</t>
         </is>
       </c>
     </row>
@@ -9216,7 +9224,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-07-06 15:33:24-05</t>
+          <t>2023-07-13 15:35:23-05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
custom fisher index calculation functionality added to the BEA data submodule. Calculate custom PCE indexes etc.
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
+++ b/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1084"/>
+  <dimension ref="A1:B1089"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9116,6 +9116,46 @@
       </c>
       <c r="B1084" t="n">
         <v>-100.128</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" s="3" t="n">
+        <v>45189</v>
+      </c>
+      <c r="B1085" t="n">
+        <v>-102.388</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" s="3" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B1086" t="n">
+        <v>-105.146</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B1087" t="n">
+        <v>-107.302</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="3" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B1088" t="n">
+        <v>-109.09</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" s="3" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B1089" t="n">
+        <v>-110.926</v>
       </c>
     </row>
   </sheetData>
@@ -9164,7 +9204,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-09-16</t>
+          <t>2023-10-23</t>
         </is>
       </c>
     </row>
@@ -9176,7 +9216,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-09-16</t>
+          <t>2023-10-23</t>
         </is>
       </c>
     </row>
@@ -9212,7 +9252,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-09-13</t>
+          <t>2023-10-18</t>
         </is>
       </c>
     </row>
@@ -9296,7 +9336,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-09-14 15:34:12-05</t>
+          <t>2023-10-19 15:34:15-05</t>
         </is>
       </c>
     </row>
@@ -9307,7 +9347,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed TGA data pull function to work with the new name change of the TGA account API endpoint.
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
+++ b/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1089"/>
+  <dimension ref="A1:B1090"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9156,6 +9156,14 @@
       </c>
       <c r="B1089" t="n">
         <v>-110.926</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" s="3" t="n">
+        <v>45224</v>
+      </c>
+      <c r="B1090" t="n">
+        <v>-113.255</v>
       </c>
     </row>
   </sheetData>
@@ -9204,7 +9212,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-10-29</t>
         </is>
       </c>
     </row>
@@ -9216,7 +9224,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-10-29</t>
         </is>
       </c>
     </row>
@@ -9252,7 +9260,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-10-18</t>
+          <t>2023-10-25</t>
         </is>
       </c>
     </row>
@@ -9336,7 +9344,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-10-19 15:34:15-05</t>
+          <t>2023-10-26 15:34:03-05</t>
         </is>
       </c>
     </row>
@@ -9347,7 +9355,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Significant upgrades to general charting tool. Can now save templates for quick reload.
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
+++ b/Generic_Macro/SavedData/RESPPLLOPNWW.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1092"/>
+  <dimension ref="A1:B1093"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9180,6 +9180,14 @@
       </c>
       <c r="B1092" t="n">
         <v>-116.882</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="3" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B1093" t="n">
+        <v>-118.699</v>
       </c>
     </row>
   </sheetData>
@@ -9228,7 +9236,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-11-15</t>
+          <t>2023-11-21</t>
         </is>
       </c>
     </row>
@@ -9240,7 +9248,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-11-15</t>
+          <t>2023-11-21</t>
         </is>
       </c>
     </row>
@@ -9276,7 +9284,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-15</t>
         </is>
       </c>
     </row>
@@ -9360,7 +9368,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-11-09 15:37:02-06</t>
+          <t>2023-11-16 15:34:06-06</t>
         </is>
       </c>
     </row>
@@ -9371,7 +9379,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>